<commit_message>
un modèle qui améliore la prise en charge des longs noms de syndicats
</commit_message>
<xml_diff>
--- a/template_2020-2021.xlsx
+++ b/template_2020-2021.xlsx
@@ -445,7 +445,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -485,7 +485,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -505,7 +505,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -597,7 +597,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -695,12 +695,13 @@
   </sheetPr>
   <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.55"/>
@@ -727,7 +728,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E2" s="2" t="str">
         <f aca="false">"Syndicat : "&amp;A74</f>
         <v>Syndicat : 01</v>
@@ -1544,7 +1545,7 @@
       </c>
       <c r="L47" s="23"/>
     </row>
-    <row r="48" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="str">
         <f aca="false">$A$74</f>
         <v>01</v>
@@ -1563,7 +1564,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="str">
         <f aca="false">$A$74</f>
         <v>01</v>
@@ -1582,7 +1583,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="12" t="str">
         <f aca="false">$A$74</f>
         <v>01</v>
@@ -1601,7 +1602,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="12" t="str">
         <f aca="false">$A$74</f>
         <v>01</v>
@@ -1620,7 +1621,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="12" t="str">
         <f aca="false">$A$74</f>
         <v>01</v>
@@ -1639,7 +1640,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="12" t="str">
         <f aca="false">$A$74</f>
         <v>01</v>
@@ -1658,7 +1659,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="12" t="str">
         <f aca="false">$A$74</f>
         <v>01</v>
@@ -1677,7 +1678,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="17" t="str">
         <f aca="false">$A$74</f>
         <v>01</v>
@@ -1935,7 +1936,7 @@
       <c r="G73" s="10"/>
       <c r="H73" s="10"/>
     </row>
-    <row r="74" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="40" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
bug dans le template
</commit_message>
<xml_diff>
--- a/template_2020-2021.xlsx
+++ b/template_2020-2021.xlsx
@@ -696,10 +696,10 @@
   <dimension ref="A1:N77"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+      <selection pane="topLeft" activeCell="J31" activeCellId="0" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.45"/>
@@ -2020,10 +2020,6 @@
     <mergeCell ref="I74:J74"/>
   </mergeCells>
   <dataValidations count="22">
-    <dataValidation allowBlank="true" error="Exemple de RNE : 1234567G" errorTitle="Saisissez un RNE" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J26:J44" type="custom">
-      <formula1>ISTEXT(_xlfn.ORG.LIBREOFFICE.REGEX(J25,"^[0-9]{7}[A-Z]$"))</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" error="Un code corps comprend trois chiffres." errorTitle="Mauvais code corps" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I25:I44" type="custom">
       <formula1>ISTEXT(_xlfn.ORG.LIBREOFFICE.REGEX(I25,"[0-9]{3}"))</formula1>
       <formula2>0</formula2>
@@ -2062,10 +2058,6 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C64:C67 F64:F67" type="decimal">
       <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Exemple de RNE : 1234567G" errorTitle="Saisissez un RNE" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J25" type="custom">
-      <formula1>ISTEXT(_xlfn.ORG.LIBREOFFICE.REGEX(J25,"^[0-9]{7}[A-Z]$"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" error="C’est “M.” ou “Mme”. Pas d’abbérviation étrange." errorTitle="M. ou Mme" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B48:B55" type="custom">
@@ -2108,6 +2100,14 @@
       <formula1>ISTEXT(_xlfn.ORG.LIBREOFFICE.REGEX(A64,"^[A-Z].* \(.*\)$"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" error="Exemple de RNE : 1234567G" errorTitle="Saisissez un RNE" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J25:J30 J32:J44" type="custom">
+      <formula1>ISTEXT(_xlfn.ORG.LIBREOFFICE.REGEX(J25,"^[0-9]{7}[A-Z]$"))</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Exemple de RNE : 1234567G" errorTitle="Saisissez un RNE" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J31" type="custom">
+      <formula1>ISTEXT(_xlfn.ORG.LIBREOFFICE.REGEX(J31,"^[0-9]{7}[A-Z]$"))</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>